<commit_message>
Nuova richiesta validazione VPS, LDO e RSA
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111ABSTRACTXXX/Abstract/SAP/1.0.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111ABSTRACTXXX/Abstract/SAP/1.0.0/report-checklist.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idoqsrl-my.sharepoint.com/personal/stefano_stellari_abstract_it/Documents/OspFe/FSE 2.0/it-fse-accreditamento-main/GATEWAY/A1#111ABSTRACTXXX/Abstract/SAP/1.0.0/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="781" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2FE41B4-E193-406A-BB47-EE911A7C4075}"/>
+  <xr:revisionPtr revIDLastSave="844" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8E9AB18-FAA9-49D7-B7C7-CA97F116D8D5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2338,13 +2338,13 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-12-14T15:28:26Z</t>
-  </si>
-  <si>
-    <t>537838f3eaefa3bc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.bb9488e37db083c329ee558bd1dc50426d94c68ea83a2313b8d4361c17b8fd84.265878de88^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-05-06T14:09:56Z</t>
+  </si>
+  <si>
+    <t>e09c6c5b5d7b5d5e</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.ca15363d6773938572954a07aba6abac6510c9252d5f8fb7f63ed6e16a926aaf.791286086b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -2487,13 +2487,13 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2023-12-22T10:19:25Z</t>
-  </si>
-  <si>
-    <t>019853fee0782b81</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.50518d58bb563ad3e0aab7832c43b12a3f74f5cd9ae846c2248dec3eda1190fa.0a761c4c49^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2024-05-06T08:53:29Z</t>
+  </si>
+  <si>
+    <t>3082d58622e4713f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.6e82849373276404a970431372c282af45e9d20be1d0c0d8617e9314ec0510d7.d4dfc1fe3d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT2</t>
@@ -2572,10 +2572,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_LDO_KO</t>
   </si>
   <si>
-    <t>2024-01-18T14:18:54Z</t>
-  </si>
-  <si>
-    <t>f36358e75feb54fb</t>
+    <t>2024-05-06T14:17:14Z</t>
+  </si>
+  <si>
+    <t>4fa286093f8d2d9b</t>
   </si>
   <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
@@ -2611,10 +2611,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_VPS_KO</t>
   </si>
   <si>
-    <t>2024-01-18T14:34:45Z</t>
-  </si>
-  <si>
-    <t>8e73b311c76aa408</t>
+    <t>2024-05-06T09:07:51Z</t>
+  </si>
+  <si>
+    <t>003e2a1f51b6aa33</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LAB_KO</t>
@@ -2669,10 +2669,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_LDO_KO</t>
   </si>
   <si>
-    <t>2024-01-18T14:26:06Z</t>
-  </si>
-  <si>
-    <t>bf0c6c7d41ae0659</t>
+    <t>2024-05-06T14:23:52Z</t>
+  </si>
+  <si>
+    <t>c9cd18033b8694b9</t>
   </si>
   <si>
     <t>/msg/jwt-validation: (Status 403)Il campo action_id non Ã¨ corretto</t>
@@ -2702,10 +2702,10 @@
     <t>VALIDAZIONE_TOKEN_JWT_CAMPO_VPS_KO</t>
   </si>
   <si>
-    <t>2024-01-18T14:41:02Z</t>
-  </si>
-  <si>
-    <t>71d470f2a326cc72</t>
+    <t>2024-05-06T09:14:31Z</t>
+  </si>
+  <si>
+    <t>7bde56d9133fd099</t>
   </si>
   <si>
     <t>VALIDAZIONE_LAB_TIMEOUT</t>
@@ -3551,7 +3551,7 @@
     <t>07e3a45970d7cdf4</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.5f873f80e366db5df437aa571aa9dbeb02199d99cd74217fac5f801bd3df5f3a.ae73035198^^^^urn:ihe:iti:xdw:20</t>
+    <t>2.16.840.1.113883.2.9.2.80.3.1.4.4.5f873f80e366db5df437aa571aa9dbeb02199d99cd74217fac5f801bd3df5f3a.ae73035198^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RSA_CT2</t>
@@ -7128,7 +7128,7 @@
   <dimension ref="A1:T992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="190" topLeftCell="B215" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="190" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
       <selection pane="bottomRight"/>
       <selection pane="bottomLeft" activeCell="A191" sqref="A191"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
@@ -13539,7 +13539,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="191" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="191" spans="1:20" ht="152.25">
       <c r="A191" s="20">
         <v>6</v>
       </c>
@@ -13556,9 +13556,9 @@
         <v>420</v>
       </c>
       <c r="F191" s="23">
-        <v>45274</v>
-      </c>
-      <c r="G191" s="23" t="s">
+        <v>45418</v>
+      </c>
+      <c r="G191" s="24" t="s">
         <v>421</v>
       </c>
       <c r="H191" s="24" t="s">
@@ -14115,7 +14115,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="207" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="207" spans="1:20" ht="137.25">
       <c r="A207" s="20">
         <v>24</v>
       </c>
@@ -14132,7 +14132,7 @@
         <v>459</v>
       </c>
       <c r="F207" s="23">
-        <v>45282</v>
+        <v>45418</v>
       </c>
       <c r="G207" s="24" t="s">
         <v>460</v>
@@ -14315,7 +14315,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="212" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="212" spans="1:20" ht="152.25">
       <c r="A212" s="20">
         <v>29</v>
       </c>
@@ -14332,7 +14332,7 @@
         <v>470</v>
       </c>
       <c r="F212" s="23">
-        <v>45309</v>
+        <v>45418</v>
       </c>
       <c r="G212" s="24" t="s">
         <v>472</v>
@@ -14563,7 +14563,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="218" spans="1:20" ht="150.75" hidden="1" thickBot="1">
+    <row r="218" spans="1:20" ht="152.25">
       <c r="A218" s="20">
         <v>35</v>
       </c>
@@ -14580,7 +14580,7 @@
         <v>470</v>
       </c>
       <c r="F218" s="23">
-        <v>45309</v>
+        <v>45418</v>
       </c>
       <c r="G218" s="24" t="s">
         <v>485</v>
@@ -14653,7 +14653,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="220" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="220" spans="1:20" ht="152.25">
       <c r="A220" s="20">
         <v>37</v>
       </c>
@@ -14670,7 +14670,7 @@
         <v>488</v>
       </c>
       <c r="F220" s="23">
-        <v>45309</v>
+        <v>45418</v>
       </c>
       <c r="G220" s="24" t="s">
         <v>490</v>
@@ -14901,7 +14901,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="226" spans="1:20" ht="165.75" hidden="1" thickBot="1">
+    <row r="226" spans="1:20" ht="152.25">
       <c r="A226" s="20">
         <v>43</v>
       </c>
@@ -14918,7 +14918,7 @@
         <v>488</v>
       </c>
       <c r="F226" s="23">
-        <v>45309</v>
+        <v>45418</v>
       </c>
       <c r="G226" s="24" t="s">
         <v>501</v>
@@ -15109,7 +15109,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="231" spans="1:20" ht="60.75">
+    <row r="231" spans="1:20" ht="60.75" hidden="1">
       <c r="A231" s="20">
         <v>48</v>
       </c>
@@ -18693,7 +18693,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="331" spans="1:20" ht="165" customHeight="1">
+    <row r="331" spans="1:20" ht="165" hidden="1" customHeight="1">
       <c r="A331" s="20">
         <v>148</v>
       </c>
@@ -18731,7 +18731,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="332" spans="1:20" ht="165" customHeight="1">
+    <row r="332" spans="1:20" ht="165" hidden="1" customHeight="1">
       <c r="A332" s="20">
         <v>149</v>
       </c>
@@ -18769,7 +18769,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="333" spans="1:20" ht="167.25">
+    <row r="333" spans="1:20" ht="167.25" hidden="1">
       <c r="A333" s="20">
         <v>150</v>
       </c>
@@ -18807,7 +18807,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="334" spans="1:20" ht="106.5">
+    <row r="334" spans="1:20" ht="106.5" hidden="1">
       <c r="A334" s="20">
         <v>151</v>
       </c>
@@ -18845,7 +18845,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="335" spans="1:20" ht="121.5">
+    <row r="335" spans="1:20" ht="121.5" hidden="1">
       <c r="A335" s="20">
         <v>152</v>
       </c>
@@ -18883,7 +18883,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="336" spans="1:20" ht="121.5">
+    <row r="336" spans="1:20" ht="121.5" hidden="1">
       <c r="A336" s="20">
         <v>153</v>
       </c>
@@ -18921,7 +18921,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="337" spans="1:20" ht="121.5">
+    <row r="337" spans="1:20" ht="121.5" hidden="1">
       <c r="A337" s="20">
         <v>154</v>
       </c>
@@ -18959,7 +18959,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="338" spans="1:20" ht="121.5">
+    <row r="338" spans="1:20" ht="121.5" hidden="1">
       <c r="A338" s="20">
         <v>155</v>
       </c>
@@ -18997,7 +18997,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="339" spans="1:20" ht="121.5">
+    <row r="339" spans="1:20" ht="121.5" hidden="1">
       <c r="A339" s="20">
         <v>156</v>
       </c>
@@ -19035,7 +19035,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="340" spans="1:20" ht="121.5">
+    <row r="340" spans="1:20" ht="121.5" hidden="1">
       <c r="A340" s="20">
         <v>157</v>
       </c>
@@ -19073,7 +19073,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="341" spans="1:20" ht="121.5">
+    <row r="341" spans="1:20" ht="121.5" hidden="1">
       <c r="A341" s="20">
         <v>158</v>
       </c>
@@ -19111,7 +19111,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="342" spans="1:20" ht="106.5">
+    <row r="342" spans="1:20" ht="106.5" hidden="1">
       <c r="A342" s="20">
         <v>159</v>
       </c>
@@ -19149,7 +19149,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="343" spans="1:20" ht="106.5">
+    <row r="343" spans="1:20" ht="106.5" hidden="1">
       <c r="A343" s="20">
         <v>160</v>
       </c>
@@ -19187,7 +19187,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="344" spans="1:20" ht="121.5">
+    <row r="344" spans="1:20" ht="121.5" hidden="1">
       <c r="A344" s="20">
         <v>161</v>
       </c>
@@ -19225,7 +19225,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="345" spans="1:20" ht="121.5">
+    <row r="345" spans="1:20" ht="121.5" hidden="1">
       <c r="A345" s="20">
         <v>162</v>
       </c>
@@ -19263,7 +19263,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="346" spans="1:20" ht="121.5">
+    <row r="346" spans="1:20" ht="121.5" hidden="1">
       <c r="A346" s="20">
         <v>163</v>
       </c>
@@ -19301,7 +19301,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="347" spans="1:20" ht="121.5">
+    <row r="347" spans="1:20" ht="121.5" hidden="1">
       <c r="A347" s="20">
         <v>164</v>
       </c>
@@ -19339,7 +19339,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="348" spans="1:20" ht="121.5">
+    <row r="348" spans="1:20" ht="121.5" hidden="1">
       <c r="A348" s="20">
         <v>165</v>
       </c>
@@ -19377,7 +19377,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="349" spans="1:20" ht="121.5">
+    <row r="349" spans="1:20" ht="121.5" hidden="1">
       <c r="A349" s="20">
         <v>166</v>
       </c>
@@ -19415,7 +19415,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="350" spans="1:20" ht="121.5">
+    <row r="350" spans="1:20" ht="121.5" hidden="1">
       <c r="A350" s="20">
         <v>167</v>
       </c>
@@ -19453,7 +19453,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="351" spans="1:20" ht="121.5">
+    <row r="351" spans="1:20" ht="121.5" hidden="1">
       <c r="A351" s="20">
         <v>168</v>
       </c>
@@ -19491,7 +19491,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="352" spans="1:20" ht="121.5">
+    <row r="352" spans="1:20" ht="121.5" hidden="1">
       <c r="A352" s="20">
         <v>169</v>
       </c>
@@ -29875,6 +29875,19 @@
     </row>
   </sheetData>
   <autoFilter ref="A9:T374" xr:uid="{00000000-0009-0000-0000-000002000000}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="147"/>
+        <filter val="24"/>
+        <filter val="29"/>
+        <filter val="32"/>
+        <filter val="35"/>
+        <filter val="37"/>
+        <filter val="40"/>
+        <filter val="43"/>
+        <filter val="6"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="1">
       <filters>
         <filter val="VALIDAZIONE"/>
@@ -29882,7 +29895,9 @@
     </filterColumn>
     <filterColumn colId="2">
       <filters>
+        <filter val="LDO"/>
         <filter val="RSA"/>
+        <filter val="VPS"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>